<commit_message>
added plot labels, added some plot samples
</commit_message>
<xml_diff>
--- a/input_data/2023_GLORIA_EXIOBASE_corresp_aggr.xlsx
+++ b/input_data/2023_GLORIA_EXIOBASE_corresp_aggr.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AE5455-48E2-5647-88C5-8A764925BB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FEF41-5760-5B43-99B5-6F59A513D296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="760" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="760" windowWidth="22260" windowHeight="12640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cover" sheetId="1" r:id="rId1"/>
     <sheet name="values" sheetId="2" r:id="rId2"/>
+    <sheet name="plot_labels" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="42">
   <si>
     <t>GLORIA END_USES</t>
   </si>
@@ -117,6 +118,36 @@
   </si>
   <si>
     <t>Warning: categories might not exactly match due to different definitions (also again see GLORIA aggregation matrices of HP Wieland for double-checks@Jan)</t>
+  </si>
+  <si>
+    <t>Enduse_name</t>
+  </si>
+  <si>
+    <t>plot_label</t>
+  </si>
+  <si>
+    <t>Civil engineering except roads</t>
+  </si>
+  <si>
+    <t>Machinery and equipment</t>
+  </si>
+  <si>
+    <t>Computers and precision instruments</t>
+  </si>
+  <si>
+    <t>Electrical equipment</t>
+  </si>
+  <si>
+    <t>Motor vehicles trailers and semi.trailers</t>
+  </si>
+  <si>
+    <t>Food packaging</t>
+  </si>
+  <si>
+    <t>Printed matter and recorded_media</t>
+  </si>
+  <si>
+    <t>Furniture and other manufactured goods nec</t>
   </si>
 </sst>
 </file>
@@ -636,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC100FD6-42FF-6943-9E4B-7715F82B5590}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -809,4 +840,271 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090551AE-2BE5-9C49-8F80-7C1F5FCABBD4}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add aggregation and correspondence of GLORIA, EXIOBASE end-use shares
</commit_message>
<xml_diff>
--- a/input_data/2023_GLORIA_EXIOBASE_corresp_aggr.xlsx
+++ b/input_data/2023_GLORIA_EXIOBASE_corresp_aggr.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FEF41-5760-5B43-99B5-6F59A513D296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8540A5E3-24A3-43F4-8AFD-8977379FF4C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="760" windowWidth="22260" windowHeight="12640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3576" yWindow="756" windowWidth="22260" windowHeight="12636" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cover" sheetId="1" r:id="rId1"/>
     <sheet name="values" sheetId="2" r:id="rId2"/>
     <sheet name="plot_labels" sheetId="3" r:id="rId3"/>
+    <sheet name="aggr_GLORIA_EXIO" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="54">
   <si>
     <t>GLORIA END_USES</t>
   </si>
@@ -148,13 +149,49 @@
   </si>
   <si>
     <t>Furniture and other manufactured goods nec</t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>GLORIA sector labels</t>
+  </si>
+  <si>
+    <t>Motor vehicles</t>
+  </si>
+  <si>
+    <t>Other transport</t>
+  </si>
+  <si>
+    <t>Civil engineering</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Other products</t>
+  </si>
+  <si>
+    <t>Plot labels (tier 1 - comp. EXIO)</t>
+  </si>
+  <si>
+    <t>Plot labels (tier 2 - only GLORIA)</t>
+  </si>
+  <si>
+    <t>EXIOBASE sector labels</t>
+  </si>
+  <si>
+    <t>mapping of GLORIA to EXIOBASE</t>
+  </si>
+  <si>
+    <t>aggregation of GLORIA sectors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +206,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +225,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,13 +289,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,18 +597,18 @@
       <selection activeCell="B4" sqref="B4:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="42.83203125" customWidth="1"/>
-    <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" customWidth="1"/>
+    <col min="4" max="4" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -513,7 +624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -521,7 +632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -529,7 +640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -537,7 +648,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -545,7 +656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -553,7 +664,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -561,7 +672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -569,7 +680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -577,7 +688,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -585,7 +696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -593,7 +704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -601,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -609,7 +720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>12</v>
       </c>
@@ -617,7 +728,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -625,7 +736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>12</v>
       </c>
@@ -633,7 +744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -641,7 +752,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -649,7 +760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>12</v>
       </c>
@@ -671,13 +782,13 @@
       <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="45.77734375" customWidth="1"/>
     <col min="2" max="2" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -693,7 +804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -701,7 +812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -709,7 +820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -717,7 +828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -725,7 +836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -733,7 +844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -741,7 +852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -749,7 +860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -757,7 +868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -765,7 +876,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -773,7 +884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -781,7 +892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -789,7 +900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -797,7 +908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -805,7 +916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -813,7 +924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -821,7 +932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -829,7 +940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -846,17 +957,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090551AE-2BE5-9C49-8F80-7C1F5FCABBD4}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -864,7 +975,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -872,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -880,7 +991,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -888,7 +999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -896,7 +1007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -904,7 +1015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -912,7 +1023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -920,7 +1031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -928,7 +1039,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -936,7 +1047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -944,7 +1055,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -952,7 +1063,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -960,7 +1071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -968,7 +1079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -976,7 +1087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -984,7 +1095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -992,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1000,7 +1111,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1008,7 +1119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1016,7 +1127,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1024,7 +1135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1032,7 +1143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1048,7 +1159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1056,7 +1167,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1064,7 +1175,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1080,7 +1191,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1088,7 +1199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1096,7 +1207,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1107,4 +1218,314 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5685A612-632C-4851-91A5-07BABF5E50B8}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
+    <col min="3" max="3" width="2.21875" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="13"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="13"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="13"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="13"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="13"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="13"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="13"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>